<commit_message>
data privacy, bug fixes of special characters in data for Telegram,mba equivalent to gmba, noun extraction fix
</commit_message>
<xml_diff>
--- a/new.xlsx
+++ b/new.xlsx
@@ -25,211 +25,235 @@
     <t>Prediction Probability</t>
   </si>
   <si>
-    <t>how long is the duration of the bdva program ?</t>
-  </si>
-  <si>
-    <t>fees of fintech?</t>
+    <t>fees of bec?</t>
+  </si>
+  <si>
+    <t>do you provide scholarship for dba?</t>
+  </si>
+  <si>
+    <t>is there placements in mgb course?</t>
+  </si>
+  <si>
+    <t>how are placement in bba program?</t>
+  </si>
+  <si>
+    <t>when is the next batch starting for dmm?</t>
+  </si>
+  <si>
+    <t>what is the amount towards registration for bdva?</t>
+  </si>
+  <si>
+    <t>what is duration of dmm course?</t>
+  </si>
+  <si>
+    <t>can you arrange a call with a counsellor?</t>
+  </si>
+  <si>
+    <t>how long is the duration of the dba program ?</t>
+  </si>
+  <si>
+    <t>what is the amount towards registration for bec?</t>
+  </si>
+  <si>
+    <t>when does the new batch start of dmm?</t>
+  </si>
+  <si>
+    <t>when does the next batch start of bbc?</t>
+  </si>
+  <si>
+    <t>is there placements in dba program?</t>
+  </si>
+  <si>
+    <t>what is the eligibility criteria for getting admission in dba?</t>
+  </si>
+  <si>
+    <t>is there any entrance exam even for the dmm course?</t>
+  </si>
+  <si>
+    <t>when does the next batch start of dba?</t>
+  </si>
+  <si>
+    <t>what about placement benefit?</t>
+  </si>
+  <si>
+    <t>how are placement in mgluxm program?</t>
+  </si>
+  <si>
+    <t>can you provide placement records of mgb?</t>
+  </si>
+  <si>
+    <t>which campus is bec offered in?</t>
+  </si>
+  <si>
+    <t>when is the next batch starting for mgb?</t>
+  </si>
+  <si>
+    <t>how are placement in dmm program?</t>
+  </si>
+  <si>
+    <t>is there an entrance exam for bbc?</t>
+  </si>
+  <si>
+    <t>scholarships criteria for bec program?</t>
+  </si>
+  <si>
+    <t>do you get loan?</t>
+  </si>
+  <si>
+    <t>can i know the avg. placement package of bdva?</t>
+  </si>
+  <si>
+    <t>do they provide us with a laptop?</t>
+  </si>
+  <si>
+    <t>is there any entrance exam for the mgluxm course?</t>
+  </si>
+  <si>
+    <t>when is the next intake for emba?</t>
+  </si>
+  <si>
+    <t>does sp jain provide placement in gfmb?</t>
+  </si>
+  <si>
+    <t>does sp jain require students to take an english language test?</t>
+  </si>
+  <si>
+    <t>duration of fintech?</t>
+  </si>
+  <si>
+    <t>scholarships criteria for bba program?</t>
+  </si>
+  <si>
+    <t>can you provide placement report for mgb program?</t>
+  </si>
+  <si>
+    <t>any placement opportunities will be provided ?</t>
+  </si>
+  <si>
+    <t>do they provide laptop?</t>
+  </si>
+  <si>
+    <t>what is the admission procedure for dba?</t>
+  </si>
+  <si>
+    <t>are there placements in fintech?</t>
+  </si>
+  <si>
+    <t>what is the admission procedure for bbc?</t>
+  </si>
+  <si>
+    <t>how long is the duration of bba?</t>
+  </si>
+  <si>
+    <t>how are placement in rm program?</t>
+  </si>
+  <si>
+    <t>duration of bba?</t>
+  </si>
+  <si>
+    <t>what is the procedure for getting in the bba program?</t>
+  </si>
+  <si>
+    <t>does sp jain provide placement as part of dmm program ?</t>
+  </si>
+  <si>
+    <t>fees of bdva?</t>
+  </si>
+  <si>
+    <t>can i know the avg. placement package of bbc?</t>
+  </si>
+  <si>
+    <t>how are placement in dba program?</t>
+  </si>
+  <si>
+    <t>can you share your placement records of fintech  program ?</t>
+  </si>
+  <si>
+    <t>i don't have a passport yet, can i still apply?</t>
+  </si>
+  <si>
+    <t>are there any scholarships,waivers i can expect for the mgluxm course?</t>
   </si>
   <si>
     <t>is it possible to have a call with your executives sometime?</t>
   </si>
   <si>
-    <t>when does the new batch start of mgb?</t>
-  </si>
-  <si>
-    <t>scholarships criteria for gfmb program?</t>
-  </si>
-  <si>
-    <t>any placement opportunities will be provided ?</t>
-  </si>
-  <si>
-    <t>when is the next intake for fintech?</t>
-  </si>
-  <si>
-    <t>can you share your placement records of bba program ?</t>
-  </si>
-  <si>
-    <t>do you accept transfer students?</t>
-  </si>
-  <si>
-    <t>what is duration of bec course?</t>
-  </si>
-  <si>
-    <t>do you have placement report for bec program?</t>
-  </si>
-  <si>
-    <t>is there any scholarship for the bbc course?</t>
-  </si>
-  <si>
-    <t>which campus is gfmb offered in?</t>
-  </si>
-  <si>
-    <t>are there any scholarships, waivers i can expect for the bbc course?</t>
-  </si>
-  <si>
-    <t>can i know the avg. placement package of emba?</t>
-  </si>
-  <si>
-    <t>when does the next batch start of gmba?</t>
-  </si>
-  <si>
-    <t>what about placement benefit?</t>
-  </si>
-  <si>
-    <t>when is the next batch starting for gfmb?</t>
-  </si>
-  <si>
-    <t>i do not meet the entry requirements, can i still apply?</t>
-  </si>
-  <si>
-    <t>which course is offered in bdva?</t>
-  </si>
-  <si>
-    <t>fees of dba?</t>
-  </si>
-  <si>
-    <t>how long is the duration of the mgb program ?</t>
-  </si>
-  <si>
-    <t>which campus is mgb offered in?</t>
-  </si>
-  <si>
-    <t>can i know about its placement avg. package?</t>
-  </si>
-  <si>
-    <t>does sp jain provide placement as part of dmm program ?</t>
-  </si>
-  <si>
-    <t>what is the total amount to be paid for registration of the gfmb course?</t>
-  </si>
-  <si>
-    <t>does sp jain provide placement as part of mgb program ?</t>
-  </si>
-  <si>
-    <t>scholarships criteria for dmm program?</t>
-  </si>
-  <si>
-    <t>what is the total amount to be paid for registration of the emba course?</t>
-  </si>
-  <si>
-    <t>when does the new batch start of bec?</t>
-  </si>
-  <si>
-    <t>is loan given?</t>
-  </si>
-  <si>
-    <t>how are placement in rm program?</t>
-  </si>
-  <si>
-    <t>what is the eligibility criteria for getting admission in bba?</t>
-  </si>
-  <si>
-    <t>when does the next batch start of dmm?</t>
-  </si>
-  <si>
-    <t>are there placements in gfmb?</t>
-  </si>
-  <si>
-    <t>scholarships criteria for dba program?</t>
-  </si>
-  <si>
-    <t>are there any scholarships, waivers given for dba?</t>
-  </si>
-  <si>
-    <t>which postgraduation courses do you offer?</t>
-  </si>
-  <si>
-    <t>what is the criteria for getting admission in mgb?</t>
-  </si>
-  <si>
-    <t>may i know the requirement for the scholarships for bbc program?</t>
-  </si>
-  <si>
-    <t>what is the eligibility criteria for getting admission in emba?</t>
-  </si>
-  <si>
-    <t>does sp jain provide placement in mgluxm?</t>
-  </si>
-  <si>
-    <t>which postgraduate courses do you offer?</t>
-  </si>
-  <si>
-    <t>how are placement in dba program?</t>
-  </si>
-  <si>
-    <t>duration of rm?</t>
-  </si>
-  <si>
-    <t>may i know the requirement for the scholarships for dmm program?</t>
-  </si>
-  <si>
-    <t>do they provide laptop?</t>
-  </si>
-  <si>
-    <t>what is the total amount to be paid for registration of the bec course?</t>
-  </si>
-  <si>
-    <t>are there placements in rm?</t>
-  </si>
-  <si>
-    <t>what is the admission procedure for gfmb?</t>
-  </si>
-  <si>
-    <t>fees of gfmb?</t>
-  </si>
-  <si>
-    <t>when does the new batch start of rm?</t>
-  </si>
-  <si>
-    <t>are there any scholarships, waivers i can expect for the dba course?</t>
-  </si>
-  <si>
-    <t>when does the new batch start of bdva?</t>
-  </si>
-  <si>
-    <t>is there any entrance exam even for the bbc course?</t>
-  </si>
-  <si>
-    <t>what is the admission procedure for emba?</t>
-  </si>
-  <si>
-    <t>what is the eligibility criteria for getting admission in bec?</t>
-  </si>
-  <si>
-    <t>can i know about its placement avg. package for bba?</t>
+    <t>when is the next intake for mgb?</t>
+  </si>
+  <si>
+    <t>can i know the avg. placement package of fintech?</t>
+  </si>
+  <si>
+    <t>what is fees of gfmb course?</t>
+  </si>
+  <si>
+    <t>fees of mgluxm?</t>
+  </si>
+  <si>
+    <t>can you share your placement records of the mgb program ?</t>
+  </si>
+  <si>
+    <t>is there any entrance exam even for the bdva course?</t>
+  </si>
+  <si>
+    <t>The total fees for the program will be INR 11,90,975 (Plus applicable service tax)</t>
+  </si>
+  <si>
+    <t>There will be a merit based scholarship for applicants based on their qualification, work experience, overall profile and performance in the DBA admission interview.</t>
+  </si>
+  <si>
+    <t>We provide complete assistance for the placements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can have a word with Mr. Rxxxxx Sxxxxxx, M: +91-xxxxxxxxxx | Email id rxxxxx.sxxxxx@spjain.org. He handles all the application for the Bachelor Of Business Administration. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The next intake is of July-17 for the DMM program. Applications are open for the same. </t>
+  </si>
+  <si>
+    <t>INR 55,000</t>
   </si>
   <si>
     <t>6 months</t>
   </si>
   <si>
-    <t>The total fees for the program will be INR 7,50,000 (plus applicable taxes).</t>
-  </si>
-  <si>
     <t>Sure we will arrange a call from one of the counsellors who can help you better regarding this.</t>
   </si>
   <si>
-    <t>The next intake of MGB is of September 2017 followed by January 2018</t>
-  </si>
-  <si>
-    <t>You can have a word with Ms. Tejal Dhulla, M: 9987081818|Email id tejal.dhulla@spjain.org. She handles all the application for the GFMB. She would be your point of contact as far as GFMB @ S P Jain is concerned.</t>
-  </si>
-  <si>
-    <t>We provide complete assistance for the placements</t>
-  </si>
-  <si>
-    <t>The next intake is of June-17. Applications are open for the same. Kindly go the following link to apply: https://www.spjain.org/programs/professional/financial-technology/apply?hsCtaTracking=4451c9be-d849-43cd-84fa-5bf595971161%7Cfa02afbd-b2a9-478b-b4b9-ad7af311b47a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can have a word with Mr. Ranjeet Singh, M: +91- 81412 97131 | Email id ranjeet.singh@spjain.org. He handles all the application for the Bachelor Of Business Administration. </t>
-  </si>
-  <si>
-    <t>Yes. Students with verifiable college/university credits can join SP Jain in their second year.</t>
-  </si>
-  <si>
-    <t>3 year full time program</t>
-  </si>
-  <si>
-    <t>I would like to inform you that we have our Admissions Manager Mr. Atharv Kale, based in Mumbai.  Atharv handles all applications for BBA, BBC and BEC coming from West India. You can get in touch with him directly. His contact details are Tel no +91 9920211171, email id: atharv.kale@spjain.org. He would be your point of contact as far as BBA, BBC and BEC @ S P Jain is concerned.</t>
+    <t>3 years</t>
+  </si>
+  <si>
+    <t>﻿I would like to inform you that we have our Admissions Manager Mr. Axxxxx Kxxxx, based in Mumbai.  Axxxxx handles all applications for BBA, BBC and BEC coming from your region. You can get in touch with him directly. His contact details are Tel no +91 xxxxxxxxxx, email id: axxxxx.kxxxxx@spjain.org. He would be your point of contact as far as BBA, BBC and BEC @ S P Jain is concerned.</t>
+  </si>
+  <si>
+    <t>The next BBC batch will commence on September 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To enrol in the program, applicants must have:  
+- A Master’s degree from a recognised University or equivalent as recognised by the DBA Committee of S P Jain and
+- At least three years of experience
+An international applicant whose undergraduate and postgraduate degree is not in the medium of English will be required to take an English language test and show an acceptable score prior to course commencement.
+English Language Requirement: IELTS: 6.5/ TOEFL iBT: 70 (minimum)/Pearson Test of English: 60 (minimum)
+The Admission Committee will shortlist candidates based on several criteria, including past academic performance, work experience and other information provided to us. 
+Shortlisted candidates will be called for an interview to test the candidate's capability to complete the course. </t>
+  </si>
+  <si>
+    <t>Appear for further evaluation comprising written tests (test of reasoning, numerical ability, english comprehension), followed by 2 round of interviews to understand the statement of purpose of the student to join the program</t>
+  </si>
+  <si>
+    <t>﻿I would like to inform you that we have our Director- Professional PG Programs Dr. Rxxxxxx Rxxxx Cxxxxx, based out of Mumbai.  He handles all applications for DMM/DBA. You can get in touch with him directly. His contact details are tel no xxxxxxxxxx/xxxxxxxxxx, email id xxxxxxx.xxxxxxx@spjain.org  . He would be your point of contact as far as DBA/DMM @ S P Jain is concerned.</t>
+  </si>
+  <si>
+    <t>﻿I would like to inform you that we have our Admissions Manager Ms. Nxxxx Sxxxxx , based out of Mumbai.  She handles all applications for MGLuxM. You can get in touch with her directly. Her contact details are tel no +91 xxxxxxxxxx, email id Nxxxxx.sxxxxx@spjain.org. She would be your point of contact as far as MGLuxM @ S P Jain is concerned.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full-time placement updates from the Intakes of 2015 that graduated in 2016/17 are provided below:
+- Over 94% of students received internship offers from companies based in Middle East and Southeast Asia. 
+- Average CTC: USD 25,485
+- Top recruiters of the season were Credit Agricole, Deloitte, Genpact,  Smytten,  Fintelix, UBS, Enhance, Bayt.com, Agility Logistics, Al Seer group, Stanley Black &amp; Decker and Kuehne + Nagel. 
+You can download the placement report of 2014-17 batch at below link:
+http://cdn2.hubspot.net/hubfs/1969827/MGB-Placement-Report-of-May14-Intake.pdf?__hssc=190427892.5.1495346778271&amp;__hstc=190427892.33e733658ed7095adf355d6d87809a81.1478335842661.1495333324545.1495346778271.15&amp;__hsfp=1107886181&amp;hsCtaTracking=8ddebeec-ee0a-4cbd-8402-8969a656d200%7C55049e8f-8c08-4083-a8e3-0fbdce42ea71
+</t>
   </si>
   <si>
     <t>Scholarships are awarded based on outstanding academic achievement:
@@ -243,108 +267,81 @@
 - SPJET score above 90th percentile</t>
   </si>
   <si>
-    <t>I would like to inform you that we have our Assistant Manager- Professional Programs for EMBA Ms. Nikita Marwaha , based out of our Mumbai Campus. Ms. Nikita handles all applications for the EMBA program. You can get in touch with her directly. Her contact details are tel no 8879866774 email id nikita.marwaha@spjain.org. She would be your point of contact as far as EMBA @ S P Jain is concerned.</t>
-  </si>
-  <si>
-    <t>The next intake of GMBA is of September 2017 followed by January 2018</t>
-  </si>
-  <si>
-    <t>The next intake is of August-17. Applications are open for the same. Kindly go the following link to apply: https://docs.google.com/forms/d/e/1FAIpQLScjq_wNNNovZ4QV9gVEKv-33mlzC2DBxeBHJGbQs42VfFU9Pw/viewform?c=0andw=1and__hssc=190427892.2.1495486494703and__hstc=190427892.33e733658ed7095adf355d6d87809a81.1478335842661.1495476073256.1495486494703.23and__hsfp=1107886181andhsCtaTracking=b4b13990-4ef8-4e30-a8a3-329571ad8273%7C42a77ae5-2e66-4d05-af10-759ecf60fb66</t>
+    <t>The next intake of MGB is of September 2017 followed by January 2018</t>
+  </si>
+  <si>
+    <t>﻿I would like to inform you that we have our Admissions Manager Mr. Axxxxxx Kxxxxxx, based out of Mumbai.  He handles all applications for Digital Marketing and Metrics . You can get in touch with him directly. His contact details are tel no +91 9xxxxxxxxx, email id axxxxxx.kxxxxxx@spjain.org . He would be your point of contact as far as DMM @ S P Jain is concerned.</t>
+  </si>
+  <si>
+    <t>Yes, students need to take either the SAT or the SP Jain Entrance Test (SPJET).</t>
+  </si>
+  <si>
+    <t>Yes ,we  have tied up with certain banks who can grant you loan</t>
+  </si>
+  <si>
+    <t>﻿You can have a word with Mr. Rxxxxx Sxxxx, M: +91- xxxxxxx131 | Email id rxxxxx.sxxxx@spjain.org. He handles all the application for the Big Data and Visual Analytics Course.</t>
+  </si>
+  <si>
+    <t>No, laptop is not provided by us.</t>
+  </si>
+  <si>
+    <t>No, there is one interview round, based on interview round we will be shortlisting your profile.</t>
+  </si>
+  <si>
+    <t>The next intake of MGB is of July 2017. Applications are open for the same.</t>
+  </si>
+  <si>
+    <t>﻿You can have a word with Ms. Txxxxx Dxxxx, M: xxxxxxxxxx|Email id xxxxx.xxxxxx@spjain.org. She handles all the application for the GFMB. She would be your point of contact as far as GFMB @ S P Jain is concerned.</t>
+  </si>
+  <si>
+    <t>While SP Jain does not require students to take an English language test at the time of admission, it is a mandatory requirement for an Australian student visa to have an English language score. Full details can be found on the Australian Government Department of Immigration and Border Protection website.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To apply for the program please:
+ Submit an online application form along with the following supporting documents like:
+- CV/Resume
+- University degree transcripts
+The Admission Committee will shortlist candidates based on several criteria, including past academic performance, work experience and other information provided to us. 
+Shortlisted candidates will be called for an interview to test the candidate's capability to complete the course. </t>
+  </si>
+  <si>
+    <t>Please refer to the following link for information on the same: https://www.spjain.org/programs/undergraduate/bbc/admissions?hsCtaTracking=472995f8-e036-4aba-87cf-11b51f03bccc%7Cbf9da8cc-2723-4f1f-b398-23bc348eb077</t>
+  </si>
+  <si>
+    <t>4 year full time program</t>
+  </si>
+  <si>
+    <t>﻿You can have a word with Mr. Axxxxxx Kxxxxxx, M: +91 xxxxxxxxxx, email id axxxxxxx.kxxxxxx@spjain.org. He handles all applications for Retail Management.</t>
+  </si>
+  <si>
+    <t>Please refer to the following link for information on the same: https://www.spjain.org/programs/undergraduate/bba/admissions?hsCtaTracking=0339d6c1-a031-450b-8513-fe7f78677a77%7C7be33b32-eacf-47b3-b0bf-36c119dc31bc</t>
+  </si>
+  <si>
+    <t>The fees of the Big Data &amp; Visual Analytics Program is INR 500,000 (Plus applicable service tax)</t>
+  </si>
+  <si>
+    <t>﻿You can have a word with Mr. Mxxxxx Sxxxxx, M: +91-xxxxxxxxxx  | Email id mxxxx.sxxxx@spjain.org. He handles all the application for the Bachelor Of Business Communication.</t>
+  </si>
+  <si>
+    <t>﻿I would like to inform you that we have our Admissions Manager Mr.Nxxxxxx Gxxxx , based out of Mumbai.  He handles all applications for Fintech  . You can get in touch with him directly. His contact details are tel no +91 xxxxxxxxxx, email id nxxxx.gxxxx@spjain.org. He would be your point of contact as far as Fintech @ S P Jain is concerned.</t>
   </si>
   <si>
     <t>Yes, you can still apply. However, you will need to have a passport by August 1 in order to apply for a student visa.</t>
   </si>
   <si>
-    <t>The fees of the Big Data and Visual Analytics Program is INR 500,000 (Plus applicable service tax)</t>
-  </si>
-  <si>
-    <t>The total fees for the program will be USD 19,500 (approx INR 12-13 lacs)</t>
-  </si>
-  <si>
-    <t>The duration of MGB program is 16 months (This includes a 4 month mandatory internship)</t>
-  </si>
-  <si>
-    <t>The total fees of the program is USD 43,825 for the Sept-17 intake. And USD 44,575 for the Jan-18 intake.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Full-time placement updates from the batches of 2016 are provided below:
--The Intake witnessed 2.5-fold jump in average post-GMBA salaries as compared with the pre-GMBA salaries
--Average CTC: USD 29,233
--Top recruiters of the season were Microsoft, Unilever, TCS, Cognizant, Wipro, ITC Infotech, HP, HCL, Genpact, Deloitte, Barclays, EandY, Dell, Landmark Group, MandM, Heinz, Dunia Finance, Abbott, Maersk and KPMG. For placement report, please click on  https://cdn2.hubspot.net/hubfs/1969827/GMBA-Placement-Report.pdf </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scholarships are awarded for EMBA based on the following:
-- Academic performance
-- Financial background
-- Work experience
-- Leadership, communication and problem-solving skills
-</t>
-  </si>
-  <si>
-    <t>INR 1,43,000 has to be paid as registration fee for EMBA</t>
-  </si>
-  <si>
-    <t>The next BEC batch will commence on September 2017</t>
-  </si>
-  <si>
-    <t>Yes ,we  have tied up with certain banks who can grant you loan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can have a word with Mr. Ashutosh Kulkarni, M: +91 9702896668, email id ashutosh.kulkarni@spjain.org. He handles all applications for Retail Management. </t>
-  </si>
-  <si>
-    <t>Please refer to the following link for information on the same: https://www.spjain.org/programs/undergraduate/bba/admissions?hsCtaTracking=0339d6c1-a031-450b-8513-fe7f78677a77%7C7be33b32-eacf-47b3-b0bf-36c119dc31bc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The next intake is of July-17 for the DMM program. Applications are open for the same. </t>
-  </si>
-  <si>
-    <t>There will be a merit based scholarship for students based on their qualification, work experience and performance in the aptitude test and personal interview.</t>
-  </si>
-  <si>
-    <t>At SP Jain, we provide Bahelors of Business Administration (BBA), Bachelors of Business Communication (BBC) and Bachelors of Economics (BEC) as undergraduate courses.</t>
-  </si>
-  <si>
-    <t>The admissions team will shortlist applications based on past academic performance, aptitude test scores, work experience, extracurricular activities and other achievements.
-Shortlisted candidates are required to visit one of the evaluation centres on campus (Dubai, Mumbai, Bengaluru, New Delhi, Kolkata, Singapore or Sydney) for further evaluation. This includes writing essays, analysing case studies and panel interviews. 
-For more details on the same, refer to the below link:
-https://www.spjain.org/programs/postgraduate/mgb/admissions?hsCtaTracking=3df2ab4c-ae43-4373-8b62-f89b8ce8fb42%7C18cd3ba9-2c18-41c5-bf45-38be3e788bd7</t>
-  </si>
-  <si>
-    <t>1. Shortlisting of profiles.
-To be eligible for EMBA, candidate must have the following:
-- Bachelor's Degree
-- 5+ years of work experience 
-- Overall Profile. Candidates will be shortlisted further based on their achievements, academic record, work experience etc.
-2. Evaluation of shortlisted profiles.
-Shortlisted applications will need to go through the evaluation process in person. This involves:
-- Aptitude test 
-- Essay
-- Interview</t>
-  </si>
-  <si>
-    <t>I would like to inform you that we have our Director- Professional PG Programs Dr. Raja Roy Choudhury, based out of Mumbai.  He handles all applications for DMM/DBA. You can get in touch with him directly. His contact details are tel no 8879489681/8655502525, email id raja.royc@spjain.org  . He would be your point of contact as far as DBA/DMM @ S P Jain is concerned.</t>
-  </si>
-  <si>
-    <t>8 months</t>
-  </si>
-  <si>
-    <t>No, laptop is not provided by us.</t>
+    <t>Yes, we provide scholarship for deserving candidates. You can find complete information on the same at the following link - https://www.spjain.org/programs/postgraduate/mgluxm</t>
+  </si>
+  <si>
+    <t>﻿I would like to inform you that we have our Admissions Manager Mr.Nxxxxxx Gxxxx , based out of Mumbai.  He handles all applications for Fintech  . You can get in touch with him directly. His contact details are tel no +91 xxxxxxxxxx, email id nxxxx.gxxxx@spjain.org. He would be your point of contact as far as DMM @ S P Jain is concerned.</t>
   </si>
   <si>
     <t>The total fees for the program will be INR 14,50,000 (plus applicable taxes).</t>
   </si>
   <si>
-    <t>I would like to inform you that we have our Admissions Manager Mr. Ashutosh Kulkarni, based out of Mumbai.  He handles all applications for Digital Marketing and Metrics . You can get in touch with him directly. His contact details are tel no +91 9702896668, email id ashutosh.kulkarni@spjain.org . He would be your point of contact as far as DMM @ S P Jain is concerned.</t>
-  </si>
-  <si>
-    <t>The next intake is of July-17 for Big Data and Visual Analytics program. Applications are open for the same. K</t>
-  </si>
-  <si>
-    <t>Yes, students need to take either the SAT or the SP Jain Entrance Test (SPJET).</t>
-  </si>
-  <si>
-    <t>Students must have completed high school/secondary school/junior college or some equivalent form of secondary education and placed in the top 25% of their class.</t>
+    <t>The fee breakup comprises of a total of 9600 euros, payable in Dubai, and INR 4,60,000, payable in India.</t>
+  </si>
+  <si>
+    <t>Yes,there is a one-hour aptitude test with numerical, quantitative reasoning, mathematics and statistical components.</t>
   </si>
 </sst>
 </file>
@@ -721,511 +718,511 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1">
-        <v>12</v>
+        <v>368</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2">
-        <v>0.48</v>
+        <v>0.345</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1">
-        <v>393</v>
+        <v>524</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3">
-        <v>0.325</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
-        <v>35</v>
+        <v>199</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0.895</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1">
-        <v>604</v>
+        <v>339</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5">
-        <v>0.315</v>
+        <v>0.57125</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1">
-        <v>450</v>
+        <v>571</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6">
-        <v>0.465</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1">
-        <v>37</v>
+        <v>287</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0.255</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1">
-        <v>563</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D8">
-        <v>0.285</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1">
-        <v>55</v>
+        <v>467</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1">
-        <v>344</v>
+        <v>249</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10">
-        <v>0.615</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1">
-        <v>89</v>
+        <v>376</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D11">
-        <v>0.515</v>
+        <v>0.285</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
-        <v>107</v>
+        <v>597</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D12">
-        <v>0.775</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1">
-        <v>76</v>
+        <v>586</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D13">
-        <v>0.47</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
-        <v>627</v>
+        <v>241</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D14">
-        <v>0.48</v>
+        <v>0.835</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1">
-        <v>78</v>
+        <v>519</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15">
-        <v>0.51</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1">
-        <v>511</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D16">
-        <v>0.48</v>
+        <v>0.415</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D17">
-        <v>0.615</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1">
-        <v>58</v>
+        <v>304</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0.918236777916172</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1">
-        <v>459</v>
+        <v>151</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D19">
-        <v>0.917138668720557</v>
+        <v>0.7216666666666666</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1">
-        <v>582</v>
+        <v>487</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
         <v>75</v>
       </c>
       <c r="D20">
-        <v>0.545</v>
+        <v>0.385</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1">
-        <v>63</v>
+        <v>622</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
         <v>76</v>
       </c>
       <c r="D21">
-        <v>0.385</v>
+        <v>0.175</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1">
-        <v>631</v>
+        <v>577</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
         <v>77</v>
       </c>
       <c r="D22">
-        <v>0.215</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1">
-        <v>518</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
         <v>78</v>
       </c>
       <c r="D23">
-        <v>0.285</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1">
-        <v>208</v>
+        <v>353</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
         <v>79</v>
       </c>
       <c r="D24">
-        <v>0.645</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1">
-        <v>620</v>
+        <v>384</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D25">
-        <v>0.14</v>
+        <v>0.365</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D26">
-        <v>0.291623015873016</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1">
-        <v>32</v>
+        <v>293</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="D27">
-        <v>0.83</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1">
-        <v>163</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="D28">
-        <v>0.295</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1">
-        <v>207</v>
+        <v>139</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="D29">
-        <v>0.845</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1">
-        <v>317</v>
+        <v>566</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D30">
-        <v>0.48</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1">
-        <v>226</v>
+        <v>108</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D31">
-        <v>0.185</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1">
-        <v>601</v>
+        <v>443</v>
       </c>
       <c r="B32" t="s">
         <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D32">
-        <v>0.275</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1">
-        <v>414</v>
+        <v>344</v>
       </c>
       <c r="B33" t="s">
         <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>0.645</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1">
-        <v>194</v>
+        <v>391</v>
       </c>
       <c r="B34" t="s">
         <v>34</v>
       </c>
       <c r="C34" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="D34">
-        <v>0.91</v>
+        <v>0.5649999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1">
-        <v>324</v>
+        <v>337</v>
       </c>
       <c r="B35" t="s">
         <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D35">
-        <v>0.545</v>
+        <v>0.385</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1">
-        <v>585</v>
+        <v>492</v>
       </c>
       <c r="B36" t="s">
         <v>36</v>
       </c>
       <c r="C36" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D36">
-        <v>0.575</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1">
-        <v>437</v>
+        <v>232</v>
       </c>
       <c r="B37" t="s">
         <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D37">
-        <v>0.46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1">
-        <v>534</v>
+        <v>340</v>
       </c>
       <c r="B38" t="s">
         <v>38</v>
@@ -1234,385 +1231,385 @@
         <v>82</v>
       </c>
       <c r="D38">
-        <v>0.415</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1">
-        <v>527</v>
+        <v>396</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="C39" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="D39">
-        <v>0.29</v>
+        <v>0.918236777916172</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1">
-        <v>610</v>
+        <v>522</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D40">
-        <v>0.415</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1">
-        <v>199</v>
+        <v>395</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="D41">
-        <v>0.27</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1">
-        <v>85</v>
+        <v>352</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D42">
-        <v>0.39</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1">
-        <v>499</v>
+        <v>332</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D43">
-        <v>0.45</v>
+        <v>0.485</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1">
-        <v>423</v>
+        <v>472</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="D44">
-        <v>0.7392307692307692</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1">
-        <v>629</v>
+        <v>320</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D45">
-        <v>0.415</v>
+        <v>0.465</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="1">
-        <v>257</v>
+        <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D46">
-        <v>0.88</v>
+        <v>0.135</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="1">
-        <v>454</v>
+        <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="D47">
-        <v>0.55</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="1">
-        <v>38</v>
+        <v>279</v>
       </c>
       <c r="B48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D48">
-        <v>0.445</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="1">
-        <v>537</v>
+        <v>361</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>0.4089246031746033</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1">
-        <v>98</v>
+        <v>446</v>
       </c>
       <c r="B50" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C50" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D50">
-        <v>0.225</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="1">
-        <v>342</v>
+        <v>530</v>
       </c>
       <c r="B51" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C51" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D51">
-        <v>0.385</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="1">
-        <v>127</v>
+        <v>535</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="C52" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>0.855</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="1">
-        <v>458</v>
+        <v>425</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="C53" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D53">
-        <v>0.835</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="1">
-        <v>439</v>
+        <v>125</v>
       </c>
       <c r="B54" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C54" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="D54">
-        <v>0.4</v>
+        <v>0.3222261904761905</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="1">
-        <v>434</v>
+        <v>342</v>
       </c>
       <c r="B55" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D55">
-        <v>0.385</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="1">
-        <v>603</v>
+        <v>142</v>
       </c>
       <c r="B56" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C56" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D56">
-        <v>0.35</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="1">
-        <v>248</v>
+        <v>103</v>
       </c>
       <c r="B57" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C57" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="D57">
-        <v>0.245</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="1">
-        <v>597</v>
+        <v>230</v>
       </c>
       <c r="B58" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C58" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="D58">
-        <v>0.295</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="1">
-        <v>75</v>
+        <v>564</v>
       </c>
       <c r="B59" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C59" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="D59">
-        <v>0.415</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="1">
-        <v>502</v>
+        <v>406</v>
       </c>
       <c r="B60" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C60" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D60">
-        <v>0.345</v>
+        <v>0.224186507936508</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="1">
-        <v>456</v>
+        <v>154</v>
       </c>
       <c r="B61" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="C61" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>0.395</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="1">
-        <v>371</v>
+        <v>412</v>
       </c>
       <c r="B62" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C62" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D62">
-        <v>0.525</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="1">
-        <v>495</v>
+        <v>208</v>
       </c>
       <c r="B63" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C63" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>0.535</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="1">
-        <v>118</v>
+        <v>200</v>
       </c>
       <c r="B64" t="s">
         <v>19</v>
       </c>
       <c r="C64" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D64">
-        <v>0.917138668720557</v>
+        <v>0.918236777916172</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="1">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="B65" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C65" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="D65">
-        <v>0.78</v>
+        <v>0.46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>